<commit_message>
working on making the program more user friendly
</commit_message>
<xml_diff>
--- a/justptx200nM.xlsx
+++ b/justptx200nM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feroze\Google Drive\DUKE 2016-2020\AxoSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4C6030-6902-46B8-BCDE-7477F0A3F308}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A710AD9-78CD-4173-9463-AD2BFF5D279B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="6138" windowHeight="3756" xr2:uid="{A0EB91B6-F008-481E-A79D-3CC2F41957E3}"/>
   </bookViews>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD70D563-6EF1-44F0-8488-9B55793E55B8}">
   <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D26" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>